<commit_message>
Added all imports and visualization of matriculas
</commit_message>
<xml_diff>
--- a/DATOS/grupos.xlsx
+++ b/DATOS/grupos.xlsx
@@ -58,7 +58,23 @@
     <t xml:space="preserve">mañana</t>
   </si>
   <si>
-    <t xml:space="preserve">50659,50660,50661</t>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">50659,50660,50661,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">50658</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Si</t>
@@ -86,7 +102,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -113,6 +129,11 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="3">
@@ -192,12 +213,13 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="12.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.12"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
REQ Asignar grupo a asignatura
</commit_message>
<xml_diff>
--- a/DATOS/grupos.xlsx
+++ b/DATOS/grupos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
   <si>
     <t xml:space="preserve">curso</t>
   </si>
@@ -56,25 +56,6 @@
   </si>
   <si>
     <t xml:space="preserve">mañana</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">50659,50660,50661,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">50658</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">Si</t>
@@ -102,7 +83,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -128,26 +109,14 @@
       <sz val="8"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFCC"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -189,8 +158,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -213,13 +182,12 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.3"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -270,17 +238,17 @@
       <c r="E2" s="0" t="n">
         <v>2020</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>12</v>
+      <c r="F2" s="0" t="n">
+        <v>50658</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>100</v>
@@ -291,7 +259,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>11</v>
@@ -303,16 +271,16 @@
         <v>2020</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>50660</v>
+        <v>50662</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J3" s="0" t="n">
         <v>100</v>
@@ -323,7 +291,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>11</v>
@@ -335,16 +303,16 @@
         <v>2020</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>50661</v>
+        <v>50658</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J4" s="0" t="n">
         <v>100</v>
@@ -355,10 +323,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>17</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>18</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>1041</v>
@@ -367,16 +335,16 @@
         <v>2020</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>50659</v>
+        <v>50658</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J5" s="0" t="n">
         <v>100</v>

</xml_diff>